<commit_message>
New cucumber scenarios, data driven with excel file
</commit_message>
<xml_diff>
--- a/src/main/java/com/automationpractice/testdata/testData.xlsx
+++ b/src/main/java/com/automationpractice/testdata/testData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9200" yWindow="12260" windowWidth="24780" windowHeight="20280" tabRatio="500"/>
+    <workbookView xWindow="30540" yWindow="11500" windowWidth="24780" windowHeight="20280" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="credentials" sheetId="1" r:id="rId1"/>
+    <sheet name="account_creation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>password</t>
   </si>
@@ -31,6 +32,63 @@
   </si>
   <si>
     <t>gdadald9@gmail.com</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>birthDay</t>
+  </si>
+  <si>
+    <t>birthMonth</t>
+  </si>
+  <si>
+    <t>birthYear</t>
+  </si>
+  <si>
+    <t>newsletters</t>
+  </si>
+  <si>
+    <t>offers</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Mrs</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -89,7 +147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -98,6 +156,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -432,7 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
@@ -480,4 +539,114 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4">
+        <v>123456</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4">
+        <v>3</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1990</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>